<commit_message>
Enhancement Added for Higher Version of Android
</commit_message>
<xml_diff>
--- a/Test Data/TestData.xlsx
+++ b/Test Data/TestData.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="19">
   <si>
     <t xml:space="preserve">DeviceName</t>
   </si>
@@ -34,7 +34,7 @@
     <t xml:space="preserve">apkPath</t>
   </si>
   <si>
-    <t xml:space="preserve">appPackageName</t>
+    <t xml:space="preserve">ws.e2m.millenia</t>
   </si>
   <si>
     <t xml:space="preserve">activityName</t>
@@ -46,28 +46,37 @@
     <t xml:space="preserve">password</t>
   </si>
   <si>
-    <t xml:space="preserve">Moto G</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TA9330AB3A</t>
+    <t xml:space="preserve">Galaxy S6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">03157df33b8e2440</t>
+  </si>
+  <si>
+    <t xml:space="preserve">7.0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">/APP's/e2m_lacity_V4.8.0.apk</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ws.e2m.lacity</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ws.e2m.main.screens.SplashScreen</t>
+  </si>
+  <si>
+    <t xml:space="preserve">brucewills@yopmail.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">#e2m321</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nexus 5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">192.168.58.101:5555</t>
   </si>
   <si>
     <t xml:space="preserve">5.1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">/APP's/e2m_Generic_V4.7.0_sql.apk</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ws.e2m.main</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ws.e2m.main.screens.SplashScreen</t>
-  </si>
-  <si>
-    <t xml:space="preserve">kevinms@yopmail.com</t>
-  </si>
-  <si>
-    <t xml:space="preserve">#e2m321</t>
   </si>
 </sst>
 </file>
@@ -78,7 +87,7 @@
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="@"/>
   </numFmts>
-  <fonts count="11">
+  <fonts count="12">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -127,7 +136,7 @@
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
-      <name val="Menlo-Regular"/>
+      <name val="Arial"/>
       <family val="0"/>
       <charset val="1"/>
     </font>
@@ -143,6 +152,13 @@
       <sz val="11"/>
       <color rgb="FF2A00FF"/>
       <name val="Monaco"/>
+      <family val="0"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Menlo-Regular"/>
       <family val="0"/>
       <charset val="1"/>
     </font>
@@ -203,7 +219,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -232,7 +248,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -245,6 +261,10 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="165" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -325,24 +345,24 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:N2"/>
+  <dimension ref="A1:N3"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="B2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="topLeft" activeCell="C1" activeCellId="0" sqref="C1"/>
-      <selection pane="bottomLeft" activeCell="H2" activeCellId="0" sqref="H2"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="bottomLeft" activeCell="D5" activeCellId="0" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="19.35"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="25.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="13.74"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="19.86"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="17.06"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="51.18"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="48.62"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="19.22"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="42.27"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="11.45"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="25.86"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="34.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="24.19"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="11.07"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="9" style="1" width="11.52"/>
   </cols>
   <sheetData>
@@ -391,28 +411,61 @@
       <c r="D2" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="E2" s="7" t="s">
+      <c r="E2" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="F2" s="7" t="s">
+      <c r="F2" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="G2" s="7" t="s">
+      <c r="G2" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="H2" s="7" t="s">
+      <c r="H2" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="I2" s="10"/>
-      <c r="J2" s="10"/>
-      <c r="K2" s="10"/>
-      <c r="L2" s="10"/>
-      <c r="M2" s="10"/>
-      <c r="N2" s="10"/>
+      <c r="I2" s="11"/>
+      <c r="J2" s="11"/>
+      <c r="K2" s="11"/>
+      <c r="L2" s="11"/>
+      <c r="M2" s="11"/>
+      <c r="N2" s="11"/>
+    </row>
+    <row r="3" customFormat="false" ht="24.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="B3" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="C3" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="D3" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="E3" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="F3" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="G3" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="H3" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="I3" s="11"/>
+      <c r="J3" s="11"/>
+      <c r="K3" s="11"/>
+      <c r="L3" s="11"/>
+      <c r="M3" s="11"/>
+      <c r="N3" s="11"/>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="G2" r:id="rId1" display="kevinms@yopmail.com"/>
+    <hyperlink ref="G2" r:id="rId1" display="brucewills@yopmail.com"/>
+    <hyperlink ref="G3" r:id="rId2" display="brucewills@yopmail.com"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>